<commit_message>
Updated Power Board BOM
</commit_message>
<xml_diff>
--- a/BOM/BOM_PowerBoard_V5.xlsx
+++ b/BOM/BOM_PowerBoard_V5.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tom_Mac/Documents/GitHub/rover-hardware/BOM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riley\USST\rover-hardware\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F883581-8A69-7A42-A5CA-7AE448C14A69}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5B9874-1614-489D-B01E-319F83BAC8EB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{707F39ED-FB34-4E84-8EC1-DB542E47F720}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15996" xr2:uid="{707F39ED-FB34-4E84-8EC1-DB542E47F720}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$2:$H$51</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$2:$H$55</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -26,6 +26,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="113">
   <si>
     <t>Description</t>
   </si>
@@ -170,15 +171,6 @@
     <t>https://www.digikey.ca/product-detail/en/kemet/C1210C682KGRAC7800/399-13497-1-ND/6126233</t>
   </si>
   <si>
-    <t>CONN USB A STACKED PCB R/A</t>
-  </si>
-  <si>
-    <t>33UBAR-TSN1R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/product-detail/en/conec/33UBAR-TSN1R/626-1610-ND/3534026</t>
-  </si>
-  <si>
     <t>CAP CER 1UF 25V X7R 0805</t>
   </si>
   <si>
@@ -200,36 +192,12 @@
     <t>https://www.digikey.ca/product-detail/en/renesas-electronics-america/R7FS128783A01CFJ-AA1/R7FS128783A01CFJ-AA1-ND/7670041</t>
   </si>
   <si>
-    <t>fuse</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/product-detail/en/phoenix-contact/1984617/277-1721-ND/950849</t>
-  </si>
-  <si>
-    <t>TERM BLOCK 6POS 45DEG 3.5MM PCB</t>
-  </si>
-  <si>
     <t>MCU LR</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/product-detail/en/phoenix-contact/1988998/277-1783-ND/950911</t>
-  </si>
-  <si>
-    <t>TERM BLOCK 2POS 45DEG 3.5MM PCB</t>
-  </si>
-  <si>
     <t>Else</t>
   </si>
   <si>
-    <t>FUSE BOARD MOUNT 80A 75VDC</t>
-  </si>
-  <si>
-    <t>0881080.UR</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/product-detail/en/littelfuse-inc/0881080.UR/F9971CT-ND/6817777</t>
-  </si>
-  <si>
     <t>No extra components</t>
   </si>
   <si>
@@ -248,12 +216,6 @@
     <t>I would advise a 28V zener. You don't want to lose all your power, just the dangerous values</t>
   </si>
   <si>
-    <t>While this is great, we already have one that is close to the battery. I don't think they are necessary</t>
-  </si>
-  <si>
-    <t>Please get 90 degree connectors</t>
-  </si>
-  <si>
     <t>I would advise against using this guy. I would use the MCU found on arduinos so you can upload the bootloader</t>
   </si>
   <si>
@@ -281,9 +243,6 @@
     <t>22pf capacitor</t>
   </si>
   <si>
-    <t>Look to see if we already have them</t>
-  </si>
-  <si>
     <t>Sensing</t>
   </si>
   <si>
@@ -306,6 +265,114 @@
   </si>
   <si>
     <t>Use this with the above current sense IC to measure up to 100A</t>
+  </si>
+  <si>
+    <t>we have 2 in a kit</t>
+  </si>
+  <si>
+    <t>whole drawer of these</t>
+  </si>
+  <si>
+    <t>Need some</t>
+  </si>
+  <si>
+    <t>CONN HEADER SMD 7POS 2MM (JST)</t>
+  </si>
+  <si>
+    <t>B7B-PH-SM4-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/jst-sales-america-inc/B7B-PH-SM4-TB-LF-SN/455-1739-1-ND/926836</t>
+  </si>
+  <si>
+    <t>SENSOR ANALOG -40C-125C SOT23-3</t>
+  </si>
+  <si>
+    <t>MCP9700T-E/TT</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/microchip-technology/MCP9700T-E-TT/MCP9700T-E-TTCT-ND/1212545</t>
+  </si>
+  <si>
+    <t>Newly added</t>
+  </si>
+  <si>
+    <t>Already have</t>
+  </si>
+  <si>
+    <t>CONN PWR JACK 1.35X3.5MM SOLDER</t>
+  </si>
+  <si>
+    <t>PJ-007</t>
+  </si>
+  <si>
+    <t>5v Barrels</t>
+  </si>
+  <si>
+    <t>temperature</t>
+  </si>
+  <si>
+    <t>12v Barrels</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/cui-inc/PJ-007/CP-2519-ND/263523</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/wurth-electronics-inc/694101308002/732-5920-ND/5047519</t>
+  </si>
+  <si>
+    <t>CONN PWR JACK 0.7X2.35MM SOLDER</t>
+  </si>
+  <si>
+    <t>CONN RCPT USB3.0 TYPEA 9POS R/A</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/molex-llc/0483930003/WM10413CT-ND/4701505</t>
+  </si>
+  <si>
+    <t>TERM BLK 6P SIDE ENT 5.08MM PCB</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/phoenix-contact/1730434/277-6363-ND/2511048</t>
+  </si>
+  <si>
+    <t>TERM BLK 2P SIDE ENT 5.08MM PCB</t>
+  </si>
+  <si>
+    <t>TERM BLK 2P TOP ENTRY 2.5MM PCB</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12v Vertical</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/phoenix-contact/1770953/277-2086-1-ND/2192496</t>
+  </si>
+  <si>
+    <t>TERM BLK 4P SIDE ENT 5.08MM PCB</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/phoenix-contact/1730418/277-6574-ND/770182</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20A Arm </t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/weidm-ller/1330710000/281-4008-ND/5997481</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mosfets </t>
+  </si>
+  <si>
+    <t>GPIO</t>
+  </si>
+  <si>
+    <t>depends on what are left for AtMega pins</t>
+  </si>
+  <si>
+    <t>To Be Done</t>
+  </si>
+  <si>
+    <t>Zener Diode calculation</t>
   </si>
 </sst>
 </file>
@@ -313,8 +380,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -428,7 +495,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -456,6 +523,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -488,7 +573,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -505,7 +590,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -517,27 +602,45 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="8" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="2"/>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="12" fillId="5" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="2" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -857,42 +960,46 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:J65"/>
+  <dimension ref="A2:K69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" customWidth="1"/>
-    <col min="2" max="2" width="43.5" customWidth="1"/>
-    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.109375" customWidth="1"/>
+    <col min="2" max="2" width="43.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.77734375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="28.33203125" customWidth="1"/>
     <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" ht="24">
-      <c r="B2" s="18" t="s">
+    <row r="2" spans="1:11" ht="23.4">
+      <c r="B2" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="19"/>
+      <c r="C2" s="21"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="19">
+    <row r="3" spans="1:11" ht="18">
       <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="19">
+      <c r="I3" s="26"/>
+      <c r="J3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="18">
       <c r="B4" s="9" t="s">
         <v>10</v>
       </c>
@@ -901,10 +1008,14 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="19">
+        <v>54</v>
+      </c>
+      <c r="I4" s="28"/>
+      <c r="J4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="18">
       <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
@@ -912,26 +1023,38 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="21">
+    <row r="6" spans="1:11" ht="21">
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" ht="19">
+      <c r="I6" t="s">
+        <v>111</v>
+      </c>
+      <c r="J6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="18">
       <c r="B7" s="9" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="10">
-        <f>SUM(G11:G43)</f>
-        <v>112.16999999999999</v>
+        <f>SUM(G11:G47)</f>
+        <v>105.38999999999999</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>
       <c r="G7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" ht="19">
+      <c r="J7" t="s">
+        <v>109</v>
+      </c>
+      <c r="K7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="18">
       <c r="B8" s="9" t="s">
         <v>9</v>
       </c>
@@ -940,8 +1063,11 @@
       <c r="E8" s="5"/>
       <c r="F8" s="6"/>
       <c r="G8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="17">
+      <c r="J8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="17.399999999999999">
       <c r="B9" s="7"/>
       <c r="C9" s="8"/>
       <c r="D9" s="1"/>
@@ -949,7 +1075,7 @@
       <c r="F9" s="6"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:10" ht="19">
+    <row r="10" spans="1:11" ht="18">
       <c r="B10" s="11" t="s">
         <v>0</v>
       </c>
@@ -972,43 +1098,43 @@
         <v>2</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="16">
-      <c r="B11" s="12" t="s">
+    <row r="11" spans="1:11" ht="15.6">
+      <c r="B11" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="35">
         <v>5</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="36">
         <v>0.65</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="36">
         <f>E11*F11</f>
         <v>3.25</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="20" t="s">
-        <v>70</v>
+      <c r="I11" s="38" t="s">
+        <v>59</v>
       </c>
       <c r="J11" s="15" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="16">
+    <row r="12" spans="1:11" ht="15.6">
       <c r="B12" s="12" t="s">
         <v>24</v>
       </c>
@@ -1025,7 +1151,7 @@
         <v>35.479999999999997</v>
       </c>
       <c r="G12" s="13">
-        <f t="shared" ref="G12:G40" si="0">E12*F12</f>
+        <f t="shared" ref="G12:G51" si="0">E12*F12</f>
         <v>35.479999999999997</v>
       </c>
       <c r="H12" s="12"/>
@@ -1034,7 +1160,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:11">
       <c r="A13" s="16"/>
       <c r="B13" s="16" t="s">
         <v>28</v>
@@ -1051,7 +1177,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13" s="16" t="s">
+      <c r="H13" s="27" t="s">
         <v>27</v>
       </c>
       <c r="I13" s="16"/>
@@ -1059,7 +1185,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="16">
+    <row r="14" spans="1:11" ht="15.6">
       <c r="B14" s="12"/>
       <c r="C14" s="12"/>
       <c r="D14" s="12"/>
@@ -1070,198 +1196,181 @@
         <v>0</v>
       </c>
       <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
-      <c r="J14" s="12"/>
-    </row>
-    <row r="15" spans="1:10" ht="16">
-      <c r="B15" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>63</v>
-      </c>
+      <c r="I14" s="18"/>
+      <c r="J14" s="15"/>
+    </row>
+    <row r="15" spans="1:11" ht="15.6">
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="12"/>
-      <c r="E15" s="12">
-        <v>1</v>
-      </c>
-      <c r="F15" s="13">
-        <v>19.77</v>
-      </c>
+      <c r="E15" s="12"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="13">
         <f t="shared" si="0"/>
-        <v>19.77</v>
-      </c>
-      <c r="H15" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="I15" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="J15" s="15" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="16">
-      <c r="B16" s="12"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+    </row>
+    <row r="16" spans="1:11" ht="15.6">
+      <c r="B16" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="12">
+        <v>2</v>
+      </c>
+      <c r="F16" s="13">
+        <v>0.74</v>
+      </c>
       <c r="G16" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H16" s="12"/>
+        <v>1.48</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="I16" s="12"/>
-      <c r="J16" s="12"/>
-    </row>
-    <row r="17" spans="2:10" ht="16">
+      <c r="J16" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="15.6">
       <c r="B17" s="12" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D17" s="12" t="s">
         <v>31</v>
       </c>
       <c r="E17" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F17" s="13">
-        <v>0.74</v>
+        <v>1.74</v>
       </c>
       <c r="G17" s="13">
         <f t="shared" si="0"/>
-        <v>1.48</v>
+        <v>1.74</v>
       </c>
       <c r="H17" s="12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="I17" s="12"/>
       <c r="J17" s="15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" ht="16">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15.6">
       <c r="B18" s="12" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E18" s="12">
         <v>1</v>
       </c>
       <c r="F18" s="13">
-        <v>1.74</v>
+        <v>1.01</v>
       </c>
       <c r="G18" s="13">
         <f t="shared" si="0"/>
-        <v>1.74</v>
+        <v>1.01</v>
       </c>
       <c r="H18" s="12" t="s">
         <v>35</v>
       </c>
       <c r="I18" s="12"/>
       <c r="J18" s="15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" ht="16">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15.6">
       <c r="B19" s="12" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>39</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D19" s="12"/>
       <c r="E19" s="12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F19" s="13">
-        <v>1.01</v>
+        <v>0.24</v>
       </c>
       <c r="G19" s="13">
         <f t="shared" si="0"/>
-        <v>1.01</v>
-      </c>
-      <c r="H19" s="12" t="s">
-        <v>35</v>
-      </c>
+        <v>0.48</v>
+      </c>
+      <c r="H19" s="12"/>
       <c r="I19" s="12"/>
       <c r="J19" s="15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="16">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="15.6">
       <c r="B20" s="12" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D20" s="12"/>
       <c r="E20" s="12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" s="13">
-        <v>0.24</v>
+        <v>1.4</v>
       </c>
       <c r="G20" s="13">
         <f t="shared" si="0"/>
-        <v>0.48</v>
+        <v>1.4</v>
       </c>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
       <c r="J20" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" ht="16">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" ht="15.6">
       <c r="B21" s="12"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
       <c r="F21" s="13"/>
-      <c r="G21" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G21" s="13"/>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
-      <c r="J21" s="12"/>
-    </row>
-    <row r="22" spans="2:10" ht="16">
-      <c r="B22" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>42</v>
-      </c>
+      <c r="J21" s="15"/>
+    </row>
+    <row r="22" spans="2:10" ht="15.6">
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
       <c r="D22" s="12"/>
-      <c r="E22" s="12">
-        <v>1</v>
-      </c>
-      <c r="F22" s="13">
-        <v>1.4</v>
-      </c>
+      <c r="E22" s="12"/>
+      <c r="F22" s="13"/>
       <c r="G22" s="13">
         <f t="shared" si="0"/>
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
-      <c r="J22" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="23" spans="2:10" ht="16">
+      <c r="J22" s="12"/>
+    </row>
+    <row r="23" spans="2:10" ht="15.6">
       <c r="B23" s="12"/>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
@@ -1273,45 +1382,50 @@
       </c>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
-      <c r="J23" s="12"/>
-    </row>
-    <row r="24" spans="2:10" ht="16">
-      <c r="B24" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12">
-        <v>2</v>
-      </c>
-      <c r="F24" s="13">
-        <v>6.15</v>
-      </c>
-      <c r="G24" s="13">
-        <f t="shared" si="0"/>
-        <v>12.3</v>
-      </c>
-      <c r="H24" s="12"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="15" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" ht="16">
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J25" s="12"/>
-    </row>
-    <row r="26" spans="2:10" ht="16">
+      <c r="J23" s="15"/>
+    </row>
+    <row r="24" spans="2:10" ht="15.6">
+      <c r="B24" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
+      <c r="F24" s="25">
+        <v>1.38</v>
+      </c>
+      <c r="G24" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="26"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="15.6">
+      <c r="B25" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="30">
+        <v>483930003</v>
+      </c>
+      <c r="D25" s="30"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="31">
+        <v>2.46</v>
+      </c>
+      <c r="G25" s="31"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="15" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="15.6">
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
@@ -1322,65 +1436,61 @@
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
     </row>
-    <row r="27" spans="2:10" ht="16">
-      <c r="B27" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="12">
-        <v>1988956</v>
-      </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12">
-        <v>10</v>
-      </c>
-      <c r="F27" s="13">
-        <v>0.65</v>
-      </c>
-      <c r="G27" s="13">
-        <f t="shared" si="0"/>
-        <v>6.5</v>
-      </c>
-      <c r="H27" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="I27" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="J27" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="2:10" ht="16">
-      <c r="B28" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C28" s="12">
-        <v>1988998</v>
-      </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12">
+    <row r="27" spans="2:10" ht="15.6">
+      <c r="B27" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="24">
+        <v>1730418</v>
+      </c>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24">
+        <v>5</v>
+      </c>
+      <c r="F27" s="25">
+        <v>4.24</v>
+      </c>
+      <c r="G27" s="25">
+        <f t="shared" si="0"/>
+        <v>21.200000000000003</v>
+      </c>
+      <c r="H27" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="I27" s="23"/>
+      <c r="J27" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="15.6">
+      <c r="B28" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C28" s="24">
+        <v>1730434</v>
+      </c>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24">
         <v>2</v>
       </c>
-      <c r="F28" s="13">
-        <v>1.9</v>
-      </c>
-      <c r="G28" s="13">
-        <f t="shared" si="0"/>
-        <v>3.8</v>
-      </c>
-      <c r="H28" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="I28" s="21" t="s">
-        <v>72</v>
-      </c>
+      <c r="F28" s="25">
+        <v>6.09</v>
+      </c>
+      <c r="G28" s="25">
+        <f t="shared" si="0"/>
+        <v>12.18</v>
+      </c>
+      <c r="H28" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="I28" s="23"/>
       <c r="J28" s="15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="2:10" ht="16">
-      <c r="B29" s="12" t="s">
-        <v>66</v>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="15.6">
+      <c r="B29" s="18" t="s">
+        <v>55</v>
       </c>
       <c r="C29" s="12">
         <v>399200502</v>
@@ -1397,224 +1507,237 @@
         <v>12.15</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="I29" s="12"/>
       <c r="J29" s="15" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="2:10" ht="16">
-      <c r="B30" s="12"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="12"/>
-      <c r="E30" s="12"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H30" s="12"/>
-      <c r="I30" s="12"/>
-      <c r="J30" s="12"/>
-    </row>
-    <row r="31" spans="2:10" ht="16">
-      <c r="B31" s="12"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="I31" s="14"/>
-      <c r="J31" s="12"/>
-    </row>
-    <row r="32" spans="2:10" ht="16">
-      <c r="B32" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32" s="16" t="s">
-        <v>52</v>
-      </c>
-      <c r="D32" s="16"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="17"/>
-      <c r="G32" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H32" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="I32" s="16" t="s">
-        <v>73</v>
-      </c>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="15" customHeight="1">
+      <c r="B30" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="25">
+        <v>1.03</v>
+      </c>
+      <c r="G30" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="I30" s="24"/>
+      <c r="J30" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="15" customHeight="1">
+      <c r="B31" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C31" s="33">
+        <v>694101308002</v>
+      </c>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="25"/>
+      <c r="G31" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="I31" s="24"/>
+      <c r="J31" s="12" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" ht="15" customHeight="1">
+      <c r="B32" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="23">
+        <v>1770953</v>
+      </c>
+      <c r="D32" s="24"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="25">
+        <v>0.88</v>
+      </c>
+      <c r="G32" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="I32" s="24"/>
       <c r="J32" s="12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" ht="16">
-      <c r="B33" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="15" customHeight="1">
+      <c r="B33" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="C33" s="23">
+        <v>1330710000</v>
+      </c>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24">
         <v>1</v>
       </c>
-      <c r="F33" s="13">
-        <v>3.07</v>
-      </c>
-      <c r="G33" s="13">
-        <f t="shared" si="0"/>
-        <v>3.07</v>
-      </c>
-      <c r="H33" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="I33" s="21" t="s">
-        <v>76</v>
-      </c>
+      <c r="F33" s="25">
+        <v>2.21</v>
+      </c>
+      <c r="G33" s="25">
+        <f t="shared" si="0"/>
+        <v>2.21</v>
+      </c>
+      <c r="H33" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="I33" s="24"/>
       <c r="J33" s="12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" ht="16">
-      <c r="B34" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="C34" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12">
-        <v>1</v>
-      </c>
-      <c r="F34" s="13">
-        <v>0.47</v>
-      </c>
-      <c r="G34" s="13">
-        <f t="shared" si="0"/>
-        <v>0.47</v>
-      </c>
-      <c r="H34" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="I34" s="21" t="s">
-        <v>80</v>
-      </c>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="15" customHeight="1">
+      <c r="B34" s="30"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="30"/>
       <c r="J34" s="12"/>
     </row>
-    <row r="35" spans="2:10" ht="16">
-      <c r="B35" s="21" t="s">
-        <v>81</v>
-      </c>
+    <row r="35" spans="2:10" ht="15.6">
+      <c r="B35" s="12"/>
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
-      <c r="E35" s="12">
-        <v>2</v>
-      </c>
+      <c r="E35" s="12"/>
       <c r="F35" s="13"/>
       <c r="G35" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H35" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="I35" s="21" t="s">
-        <v>80</v>
-      </c>
+      <c r="H35" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I35" s="14"/>
       <c r="J35" s="12"/>
     </row>
-    <row r="36" spans="2:10" ht="16">
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-    </row>
-    <row r="37" spans="2:10" ht="16">
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
+    <row r="36" spans="2:10" ht="15.6">
+      <c r="B36" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D36" s="16"/>
+      <c r="E36" s="16"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H36" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="J36" s="12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" ht="15.6">
+      <c r="B37" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>62</v>
+      </c>
       <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="13"/>
+      <c r="E37" s="12">
+        <v>1</v>
+      </c>
+      <c r="F37" s="13">
+        <v>3.07</v>
+      </c>
       <c r="G37" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H37" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
-    </row>
-    <row r="38" spans="2:10" ht="16">
-      <c r="B38" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>85</v>
+        <v>3.07</v>
+      </c>
+      <c r="H37" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="I37" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" ht="15.6">
+      <c r="B38" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>66</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="12">
         <v>1</v>
       </c>
       <c r="F38" s="13">
-        <v>4.34</v>
+        <v>0.47</v>
       </c>
       <c r="G38" s="13">
         <f t="shared" si="0"/>
-        <v>4.34</v>
-      </c>
-      <c r="H38" s="12"/>
-      <c r="I38" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="J38" s="12" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="39" spans="2:10" ht="16">
-      <c r="B39" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="C39" s="22" t="s">
-        <v>88</v>
-      </c>
+        <v>0.47</v>
+      </c>
+      <c r="H38" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="I38" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="J38" s="12"/>
+    </row>
+    <row r="39" spans="2:10" ht="15.6">
+      <c r="B39" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="12"/>
       <c r="D39" s="12"/>
       <c r="E39" s="12">
-        <v>1</v>
-      </c>
-      <c r="F39" s="13">
-        <v>4.93</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="F39" s="13"/>
       <c r="G39" s="13">
         <f t="shared" si="0"/>
-        <v>4.93</v>
-      </c>
-      <c r="H39" s="12"/>
-      <c r="I39" s="21" t="s">
-        <v>90</v>
+        <v>0</v>
+      </c>
+      <c r="H39" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="I39" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="J39" s="12"/>
     </row>
-    <row r="40" spans="2:10" ht="16">
+    <row r="40" spans="2:10" ht="15.6">
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
@@ -1628,128 +1751,195 @@
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
     </row>
-    <row r="41" spans="2:10" ht="16">
+    <row r="41" spans="2:10" ht="15.6">
       <c r="B41" s="12"/>
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
       <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="12"/>
+      <c r="G41" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H41" s="14" t="s">
+        <v>69</v>
+      </c>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
     </row>
-    <row r="42" spans="2:10" ht="16">
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
+    <row r="42" spans="2:10" ht="15.6">
+      <c r="B42" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>71</v>
+      </c>
       <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
+      <c r="E42" s="12">
+        <v>1</v>
+      </c>
+      <c r="F42" s="13">
+        <v>4.34</v>
+      </c>
+      <c r="G42" s="13">
+        <f t="shared" si="0"/>
+        <v>4.34</v>
+      </c>
       <c r="H42" s="12"/>
-      <c r="I42" s="12"/>
-      <c r="J42" s="12"/>
-    </row>
-    <row r="43" spans="2:10" ht="16">
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
+      <c r="I42" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="J42" s="15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" ht="15.6">
+      <c r="B43" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>74</v>
+      </c>
       <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
+      <c r="E43" s="12">
+        <v>1</v>
+      </c>
+      <c r="F43" s="13">
+        <v>4.93</v>
+      </c>
+      <c r="G43" s="13">
+        <f t="shared" si="0"/>
+        <v>4.93</v>
+      </c>
       <c r="H43" s="12"/>
-      <c r="I43" s="12"/>
+      <c r="I43" s="18" t="s">
+        <v>76</v>
+      </c>
       <c r="J43" s="12"/>
     </row>
-    <row r="44" spans="2:10" ht="16">
+    <row r="44" spans="2:10" ht="15.6">
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
       <c r="F44" s="13"/>
-      <c r="G44" s="13"/>
+      <c r="G44" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H44" s="12"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
     </row>
-    <row r="45" spans="2:10" ht="16">
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="13"/>
-      <c r="G45" s="13"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-    </row>
-    <row r="46" spans="2:10" ht="16">
+    <row r="45" spans="2:10" ht="15.6">
+      <c r="B45" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24"/>
+      <c r="F45" s="25">
+        <v>0.41</v>
+      </c>
+      <c r="G45" s="25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H45" s="24"/>
+      <c r="I45" s="23" t="s">
+        <v>91</v>
+      </c>
+      <c r="J45" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" ht="15.6">
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
       <c r="E46" s="12"/>
       <c r="F46" s="13"/>
-      <c r="G46" s="13"/>
+      <c r="G46" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H46" s="12"/>
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
     </row>
-    <row r="47" spans="2:10" ht="16">
+    <row r="47" spans="2:10" ht="15.6">
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
       <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
+      <c r="G47" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H47" s="12"/>
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
     </row>
-    <row r="48" spans="2:10" ht="16">
+    <row r="48" spans="2:10" ht="15.6">
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
       <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
+      <c r="G48" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H48" s="12"/>
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
     </row>
-    <row r="49" spans="2:10" ht="16">
+    <row r="49" spans="2:10" ht="15.6">
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
       <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
+      <c r="G49" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H49" s="12"/>
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
     </row>
-    <row r="50" spans="2:10" ht="16">
+    <row r="50" spans="2:10" ht="15.6">
       <c r="B50" s="12"/>
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
       <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
+      <c r="G50" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H50" s="12"/>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
     </row>
-    <row r="51" spans="2:10" ht="16">
+    <row r="51" spans="2:10" ht="15.6">
       <c r="B51" s="12"/>
       <c r="C51" s="12"/>
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
       <c r="F51" s="13"/>
-      <c r="G51" s="13"/>
+      <c r="G51" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="H51" s="12"/>
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
     </row>
-    <row r="52" spans="2:10" ht="16">
+    <row r="52" spans="2:10" ht="15.6">
       <c r="B52" s="12"/>
       <c r="C52" s="12"/>
       <c r="D52" s="12"/>
@@ -1760,7 +1950,7 @@
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
     </row>
-    <row r="53" spans="2:10" ht="16">
+    <row r="53" spans="2:10" ht="15.6">
       <c r="B53" s="12"/>
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
@@ -1771,7 +1961,7 @@
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
     </row>
-    <row r="54" spans="2:10" ht="16">
+    <row r="54" spans="2:10" ht="15.6">
       <c r="B54" s="12"/>
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
@@ -1782,58 +1972,104 @@
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
     </row>
-    <row r="55" spans="2:10" ht="16">
+    <row r="55" spans="2:10" ht="15.6">
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="13"/>
       <c r="G55" s="13"/>
-    </row>
-    <row r="56" spans="2:10" ht="16">
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
+    </row>
+    <row r="56" spans="2:10" ht="15.6">
+      <c r="B56" s="12"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12"/>
+      <c r="F56" s="13"/>
       <c r="G56" s="13"/>
-    </row>
-    <row r="57" spans="2:10" ht="16">
+      <c r="H56" s="12"/>
+      <c r="I56" s="12"/>
+      <c r="J56" s="12"/>
+    </row>
+    <row r="57" spans="2:10" ht="15.6">
+      <c r="B57" s="12"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="12"/>
+      <c r="E57" s="12"/>
+      <c r="F57" s="13"/>
       <c r="G57" s="13"/>
-    </row>
-    <row r="58" spans="2:10" ht="16">
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
+    </row>
+    <row r="58" spans="2:10" ht="15.6">
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="12"/>
+      <c r="E58" s="12"/>
+      <c r="F58" s="13"/>
       <c r="G58" s="13"/>
-    </row>
-    <row r="59" spans="2:10" ht="16">
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+    </row>
+    <row r="59" spans="2:10" ht="15.6">
       <c r="G59" s="13"/>
     </row>
-    <row r="60" spans="2:10" ht="16">
+    <row r="60" spans="2:10" ht="15.6">
       <c r="G60" s="13"/>
     </row>
-    <row r="61" spans="2:10" ht="16">
+    <row r="61" spans="2:10" ht="15.6">
       <c r="G61" s="13"/>
     </row>
-    <row r="62" spans="2:10" ht="16">
+    <row r="62" spans="2:10" ht="15.6">
       <c r="G62" s="13"/>
     </row>
-    <row r="63" spans="2:10" ht="16">
+    <row r="63" spans="2:10" ht="15.6">
       <c r="G63" s="13"/>
     </row>
-    <row r="64" spans="2:10" ht="16">
+    <row r="64" spans="2:10" ht="15.6">
       <c r="G64" s="13"/>
     </row>
-    <row r="65" spans="7:7" ht="16">
+    <row r="65" spans="7:7" ht="15.6">
       <c r="G65" s="13"/>
+    </row>
+    <row r="66" spans="7:7" ht="15.6">
+      <c r="G66" s="13"/>
+    </row>
+    <row r="67" spans="7:7" ht="15.6">
+      <c r="G67" s="13"/>
+    </row>
+    <row r="68" spans="7:7" ht="15.6">
+      <c r="G68" s="13"/>
+    </row>
+    <row r="69" spans="7:7" ht="15.6">
+      <c r="G69" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="J18" r:id="rId1" xr:uid="{E2202BFF-8234-441C-B81A-9025176A8C37}"/>
+    <hyperlink ref="J17" r:id="rId1" xr:uid="{E2202BFF-8234-441C-B81A-9025176A8C37}"/>
     <hyperlink ref="J13" r:id="rId2" xr:uid="{FCD0CF73-09DF-4A54-B75D-995E7B3F3273}"/>
     <hyperlink ref="J11" r:id="rId3" xr:uid="{0ADE7EEE-8E6C-4C03-A670-5F22A9A7B57F}"/>
     <hyperlink ref="J12" r:id="rId4" xr:uid="{80EAE6D4-A8C6-4FA6-8A79-35FBE448E247}"/>
-    <hyperlink ref="J17" r:id="rId5" xr:uid="{989D5D27-A0E6-4D2C-B6D9-1486A1A85D7D}"/>
-    <hyperlink ref="J20" r:id="rId6" xr:uid="{9A93B334-DB1E-47D4-9F72-6A04BEF905BE}"/>
-    <hyperlink ref="J19" r:id="rId7" xr:uid="{C146487F-8A55-47D0-81A5-1E4ACBF756C1}"/>
-    <hyperlink ref="J22" r:id="rId8" xr:uid="{74A76CE5-1740-4604-B4E9-33F5492BEEE7}"/>
-    <hyperlink ref="J24" r:id="rId9" xr:uid="{29662F87-2ACA-4BDC-AE1C-B88797824F7C}"/>
-    <hyperlink ref="J28" r:id="rId10" xr:uid="{7ED87ECA-B664-48D2-9105-BF446FC54B49}"/>
-    <hyperlink ref="J15" r:id="rId11" xr:uid="{2FD08B2F-27DE-794B-A55A-7676405C2DE2}"/>
-    <hyperlink ref="J29" r:id="rId12" xr:uid="{B64613A2-D928-794D-9322-5F41A3F75BA9}"/>
+    <hyperlink ref="J16" r:id="rId5" xr:uid="{989D5D27-A0E6-4D2C-B6D9-1486A1A85D7D}"/>
+    <hyperlink ref="J19" r:id="rId6" xr:uid="{9A93B334-DB1E-47D4-9F72-6A04BEF905BE}"/>
+    <hyperlink ref="J18" r:id="rId7" xr:uid="{C146487F-8A55-47D0-81A5-1E4ACBF756C1}"/>
+    <hyperlink ref="J20" r:id="rId8" xr:uid="{74A76CE5-1740-4604-B4E9-33F5492BEEE7}"/>
+    <hyperlink ref="J29" r:id="rId9" xr:uid="{B64613A2-D928-794D-9322-5F41A3F75BA9}"/>
+    <hyperlink ref="J42" r:id="rId10" xr:uid="{89C89E43-E61E-4599-8565-501AE9746EE6}"/>
+    <hyperlink ref="J25" r:id="rId11" xr:uid="{B438B4D8-661B-4982-8181-2CE3940B146D}"/>
+    <hyperlink ref="J28" r:id="rId12" xr:uid="{145D90CA-E61E-4FA6-B49C-9DD551BFB85B}"/>
+    <hyperlink ref="J27" r:id="rId13" xr:uid="{23C878EF-4344-44FA-B545-AB4F0628BD8E}"/>
+    <hyperlink ref="J45" r:id="rId14" xr:uid="{7597AE0D-2257-4F35-859F-75725C862BA4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="56" orientation="portrait" r:id="rId13"/>
+  <pageSetup scale="56" orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Worked on Arm BOM
</commit_message>
<xml_diff>
--- a/BOM/BOM_PowerBoard_V5.xlsx
+++ b/BOM/BOM_PowerBoard_V5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riley\USST\rover-hardware\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5B9874-1614-489D-B01E-319F83BAC8EB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B027D38-3363-45D0-979D-D53B0E4BCA0E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15996" xr2:uid="{707F39ED-FB34-4E84-8EC1-DB542E47F720}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$2:$H$55</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$2:$H$54</definedName>
   </definedNames>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="114">
   <si>
     <t>Description</t>
   </si>
@@ -180,18 +180,6 @@
     <t>https://www.digikey.ca/product-detail/en/kemet/C0805C105K3RACTU/399-8004-6-ND/3472535</t>
   </si>
   <si>
-    <t>SYNERGY MCU PLATFORM S128 256K 3</t>
-  </si>
-  <si>
-    <t>R7FS128783A01CFJ#AA1</t>
-  </si>
-  <si>
-    <t>MC</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/product-detail/en/renesas-electronics-america/R7FS128783A01CFJ-AA1/R7FS128783A01CFJ-AA1-ND/7670041</t>
-  </si>
-  <si>
     <t>MCU LR</t>
   </si>
   <si>
@@ -216,18 +204,12 @@
     <t>I would advise a 28V zener. You don't want to lose all your power, just the dangerous values</t>
   </si>
   <si>
-    <t>I would advise against using this guy. I would use the MCU found on arduinos so you can upload the bootloader</t>
-  </si>
-  <si>
     <t>IC MCU 8BIT 32KB FLASH 28DIP</t>
   </si>
   <si>
     <t>ATMEGA328-PU</t>
   </si>
   <si>
-    <t>This is the arduino MCU. Learn how to upload the bootloader here: https://www.arduino.cc/en/Tutorial/ArduinoToBreadboard</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/product-detail/en/microchip-technology/ATMEGA328-PU/ATMEGA328-PU-ND/2271026</t>
   </si>
   <si>
@@ -237,9 +219,6 @@
     <t>9B-16.000MBBK-B</t>
   </si>
   <si>
-    <t>Used for above MCU programming</t>
-  </si>
-  <si>
     <t>22pf capacitor</t>
   </si>
   <si>
@@ -270,9 +249,6 @@
     <t>we have 2 in a kit</t>
   </si>
   <si>
-    <t>whole drawer of these</t>
-  </si>
-  <si>
     <t>Need some</t>
   </si>
   <si>
@@ -373,6 +349,33 @@
   </si>
   <si>
     <t>Zener Diode calculation</t>
+  </si>
+  <si>
+    <t>Total of three</t>
+  </si>
+  <si>
+    <t>don't need an external clock</t>
+  </si>
+  <si>
+    <t>Serial port</t>
+  </si>
+  <si>
+    <t>Usb port</t>
+  </si>
+  <si>
+    <t>Arduino to usb chip</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPTC111LFBN-RC/S7009-ND/810150</t>
+  </si>
+  <si>
+    <t>CONN HDR 11POS 0.1 TIN PCB</t>
+  </si>
+  <si>
+    <t>PPTC111LFBN-RC</t>
+  </si>
+  <si>
+    <t>arduino GPIO</t>
   </si>
 </sst>
 </file>
@@ -383,7 +386,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -494,6 +497,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="9">
     <fill>
@@ -573,7 +583,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -616,13 +626,6 @@
     <xf numFmtId="165" fontId="12" fillId="5" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="2" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -641,6 +644,14 @@
     <xf numFmtId="165" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -649,6 +660,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF5050"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -960,10 +976,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:K69"/>
+  <dimension ref="A2:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -980,10 +996,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="23.4">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="21"/>
+      <c r="C2" s="37"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
@@ -994,9 +1010,9 @@
       <c r="C3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="26"/>
+      <c r="I3" s="23"/>
       <c r="J3" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="18">
@@ -1008,11 +1024,11 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="28"/>
+        <v>50</v>
+      </c>
+      <c r="I4" s="25"/>
       <c r="J4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="18">
@@ -1029,10 +1045,10 @@
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="I6" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="J6" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="18">
@@ -1040,18 +1056,18 @@
         <v>12</v>
       </c>
       <c r="C7" s="10">
-        <f>SUM(G11:G47)</f>
+        <f>SUM(G11:G46)</f>
         <v>105.38999999999999</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>
       <c r="G7" s="1"/>
-      <c r="J7" t="s">
-        <v>109</v>
+      <c r="J7" s="39" t="s">
+        <v>101</v>
       </c>
       <c r="K7" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="18">
@@ -1064,7 +1080,7 @@
       <c r="F8" s="6"/>
       <c r="G8" s="1"/>
       <c r="J8" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="17.399999999999999">
@@ -1074,6 +1090,9 @@
       <c r="E9" s="5"/>
       <c r="F9" s="6"/>
       <c r="G9" s="1"/>
+      <c r="J9" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="18">
       <c r="B10" s="11" t="s">
@@ -1098,37 +1117,37 @@
         <v>2</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J10" s="11" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.6">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="35" t="s">
+      <c r="C11" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="35" t="s">
+      <c r="D11" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="35">
+      <c r="E11" s="32">
         <v>5</v>
       </c>
-      <c r="F11" s="36">
+      <c r="F11" s="33">
         <v>0.65</v>
       </c>
-      <c r="G11" s="36">
+      <c r="G11" s="33">
         <f>E11*F11</f>
         <v>3.25</v>
       </c>
-      <c r="H11" s="37" t="s">
+      <c r="H11" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="I11" s="38" t="s">
-        <v>59</v>
+      <c r="I11" s="35" t="s">
+        <v>55</v>
       </c>
       <c r="J11" s="15" t="s">
         <v>16</v>
@@ -1151,7 +1170,7 @@
         <v>35.479999999999997</v>
       </c>
       <c r="G12" s="13">
-        <f t="shared" ref="G12:G51" si="0">E12*F12</f>
+        <f t="shared" ref="G12:G50" si="0">E12*F12</f>
         <v>35.479999999999997</v>
       </c>
       <c r="H12" s="12"/>
@@ -1177,7 +1196,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H13" s="27" t="s">
+      <c r="H13" s="24" t="s">
         <v>27</v>
       </c>
       <c r="I13" s="16"/>
@@ -1385,44 +1404,48 @@
       <c r="J23" s="15"/>
     </row>
     <row r="24" spans="2:10" ht="15.6">
-      <c r="B24" s="23" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24"/>
-      <c r="F24" s="25">
+      <c r="B24" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="22">
         <v>1.38</v>
       </c>
-      <c r="G24" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="22" t="s">
-        <v>82</v>
+      <c r="G24" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="I24" s="23"/>
+      <c r="J24" s="15" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.6">
       <c r="B25" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="30">
+        <v>88</v>
+      </c>
+      <c r="C25" s="27">
         <v>483930003</v>
       </c>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="31">
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="28">
         <v>2.46</v>
       </c>
-      <c r="G25" s="31"/>
-      <c r="H25" s="32"/>
-      <c r="I25" s="32"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="I25" s="29"/>
       <c r="J25" s="15" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="2:10" ht="15.6">
@@ -1437,60 +1460,60 @@
       <c r="J26" s="12"/>
     </row>
     <row r="27" spans="2:10" ht="15.6">
-      <c r="B27" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="C27" s="24">
+      <c r="B27" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="21">
         <v>1730418</v>
       </c>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24">
+      <c r="D27" s="21"/>
+      <c r="E27" s="21">
         <v>5</v>
       </c>
-      <c r="F27" s="25">
+      <c r="F27" s="22">
         <v>4.24</v>
       </c>
-      <c r="G27" s="25">
+      <c r="G27" s="22">
         <f t="shared" si="0"/>
         <v>21.200000000000003</v>
       </c>
-      <c r="H27" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="I27" s="23"/>
+      <c r="H27" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="I27" s="20"/>
       <c r="J27" s="15" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.6">
-      <c r="B28" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C28" s="24">
+      <c r="B28" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="C28" s="21">
         <v>1730434</v>
       </c>
-      <c r="D28" s="24"/>
-      <c r="E28" s="24">
+      <c r="D28" s="21"/>
+      <c r="E28" s="21">
         <v>2</v>
       </c>
-      <c r="F28" s="25">
+      <c r="F28" s="22">
         <v>6.09</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="22">
         <f t="shared" si="0"/>
         <v>12.18</v>
       </c>
-      <c r="H28" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="I28" s="23"/>
+      <c r="H28" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="I28" s="20"/>
       <c r="J28" s="15" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15.6">
       <c r="B29" s="18" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C29" s="12">
         <v>399200502</v>
@@ -1507,118 +1530,118 @@
         <v>12.15</v>
       </c>
       <c r="H29" s="12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="I29" s="12"/>
       <c r="J29" s="15" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15" customHeight="1">
-      <c r="B30" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="C30" s="34" t="s">
-        <v>89</v>
-      </c>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-      <c r="F30" s="25">
+      <c r="B30" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="22">
         <v>1.03</v>
       </c>
-      <c r="G30" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H30" s="23" t="s">
+      <c r="G30" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="I30" s="21"/>
+      <c r="J30" s="12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" ht="15" customHeight="1">
+      <c r="B31" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" s="30">
+        <v>694101308002</v>
+      </c>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H31" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="I31" s="21"/>
+      <c r="J31" s="12" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" ht="15" customHeight="1">
+      <c r="B32" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" s="20">
+        <v>1770953</v>
+      </c>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="22">
+        <v>0.88</v>
+      </c>
+      <c r="G32" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H32" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="I32" s="21"/>
+      <c r="J32" s="12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="15" customHeight="1">
+      <c r="B33" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="I30" s="24"/>
-      <c r="J30" s="12" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="31" spans="2:10" ht="15" customHeight="1">
-      <c r="B31" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" s="33">
-        <v>694101308002</v>
-      </c>
-      <c r="D31" s="24"/>
-      <c r="E31" s="24"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H31" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="I31" s="24"/>
-      <c r="J31" s="12" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="32" spans="2:10" ht="15" customHeight="1">
-      <c r="B32" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="C32" s="23">
-        <v>1770953</v>
-      </c>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-      <c r="F32" s="25">
-        <v>0.88</v>
-      </c>
-      <c r="G32" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H32" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="I32" s="24"/>
-      <c r="J32" s="12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" ht="15" customHeight="1">
-      <c r="B33" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="C33" s="23">
+      <c r="C33" s="20">
         <v>1330710000</v>
       </c>
-      <c r="D33" s="24"/>
-      <c r="E33" s="24">
+      <c r="D33" s="21"/>
+      <c r="E33" s="21">
         <v>1</v>
       </c>
-      <c r="F33" s="25">
+      <c r="F33" s="22">
         <v>2.21</v>
       </c>
-      <c r="G33" s="25">
+      <c r="G33" s="22">
         <f t="shared" si="0"/>
         <v>2.21</v>
       </c>
-      <c r="H33" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="I33" s="24"/>
+      <c r="H33" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="I33" s="21"/>
       <c r="J33" s="12" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="15" customHeight="1">
-      <c r="B34" s="30"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="30"/>
-      <c r="E34" s="30"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="29"/>
-      <c r="I34" s="30"/>
+      <c r="B34" s="27"/>
+      <c r="C34" s="26"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="27"/>
       <c r="J34" s="12"/>
     </row>
     <row r="35" spans="2:10" ht="15.6">
@@ -1638,104 +1661,100 @@
       <c r="J35" s="12"/>
     </row>
     <row r="36" spans="2:10" ht="15.6">
-      <c r="B36" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C36" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H36" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="I36" s="16" t="s">
+      <c r="B36" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12">
+        <v>1</v>
+      </c>
+      <c r="F36" s="13">
+        <v>3.07</v>
+      </c>
+      <c r="G36" s="13">
+        <f t="shared" si="0"/>
+        <v>3.07</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="I36" s="18"/>
+      <c r="J36" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" ht="15.6">
+      <c r="B37" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="J36" s="12" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" ht="15.6">
-      <c r="B37" s="19" t="s">
+      <c r="D37" s="27"/>
+      <c r="E37" s="27">
+        <v>1</v>
+      </c>
+      <c r="F37" s="28">
+        <v>0.47</v>
+      </c>
+      <c r="G37" s="28">
+        <f t="shared" si="0"/>
+        <v>0.47</v>
+      </c>
+      <c r="H37" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="I37" s="26"/>
+      <c r="J37" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" ht="15.6">
+      <c r="B38" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C37" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12">
-        <v>1</v>
-      </c>
-      <c r="F37" s="13">
-        <v>3.07</v>
-      </c>
-      <c r="G37" s="13">
-        <f t="shared" si="0"/>
-        <v>3.07</v>
-      </c>
-      <c r="H37" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="I37" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="J37" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" ht="15.6">
-      <c r="B38" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="C38" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12">
-        <v>1</v>
-      </c>
-      <c r="F38" s="13">
-        <v>0.47</v>
-      </c>
-      <c r="G38" s="13">
-        <f t="shared" si="0"/>
-        <v>0.47</v>
-      </c>
-      <c r="H38" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="I38" s="18" t="s">
-        <v>67</v>
-      </c>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27">
+        <v>2</v>
+      </c>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H38" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="I38" s="26"/>
       <c r="J38" s="12"/>
     </row>
     <row r="39" spans="2:10" ht="15.6">
-      <c r="B39" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="C39" s="12"/>
+      <c r="B39" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>112</v>
+      </c>
       <c r="D39" s="12"/>
-      <c r="E39" s="12">
-        <v>2</v>
-      </c>
-      <c r="F39" s="13"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="13">
+        <v>1.06</v>
+      </c>
       <c r="G39" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="I39" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="J39" s="12"/>
+        <v>113</v>
+      </c>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="40" spans="2:10" ht="15.6">
       <c r="B40" s="12"/>
@@ -1747,113 +1766,113 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H40" s="12"/>
+      <c r="H40" s="14" t="s">
+        <v>62</v>
+      </c>
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
     </row>
     <row r="41" spans="2:10" ht="15.6">
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
+      <c r="B41" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>64</v>
+      </c>
       <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="13"/>
+      <c r="E41" s="12">
+        <v>1</v>
+      </c>
+      <c r="F41" s="13">
+        <v>4.34</v>
+      </c>
       <c r="G41" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H41" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
+        <v>4.34</v>
+      </c>
+      <c r="H41" s="12"/>
+      <c r="I41" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="J41" s="15" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="42" spans="2:10" ht="15.6">
       <c r="B42" s="19" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="12">
         <v>1</v>
       </c>
       <c r="F42" s="13">
-        <v>4.34</v>
+        <v>4.93</v>
       </c>
       <c r="G42" s="13">
         <f t="shared" si="0"/>
-        <v>4.34</v>
+        <v>4.93</v>
       </c>
       <c r="H42" s="12"/>
       <c r="I42" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="J42" s="15" t="s">
-        <v>73</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="J42" s="12"/>
     </row>
     <row r="43" spans="2:10" ht="15.6">
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="12"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
+      <c r="F43" s="13"/>
+      <c r="G43" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H43" s="12"/>
+      <c r="I43" s="12"/>
+      <c r="J43" s="12"/>
+    </row>
+    <row r="44" spans="2:10" ht="15.6">
+      <c r="B44" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="C43" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12">
-        <v>1</v>
-      </c>
-      <c r="F43" s="13">
-        <v>4.93</v>
-      </c>
-      <c r="G43" s="13">
-        <f t="shared" si="0"/>
-        <v>4.93</v>
-      </c>
-      <c r="H43" s="12"/>
-      <c r="I43" s="18" t="s">
+      <c r="C44" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="J43" s="12"/>
-    </row>
-    <row r="44" spans="2:10" ht="15.6">
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H44" s="12"/>
-      <c r="I44" s="12"/>
-      <c r="J44" s="12"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="22">
+        <v>0.41</v>
+      </c>
+      <c r="G44" s="22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H44" s="21"/>
+      <c r="I44" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="J44" s="15" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="45" spans="2:10" ht="15.6">
-      <c r="B45" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C45" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="25">
-        <v>0.41</v>
-      </c>
-      <c r="G45" s="25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H45" s="24"/>
-      <c r="I45" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="J45" s="15" t="s">
-        <v>85</v>
-      </c>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
     </row>
     <row r="46" spans="2:10" ht="15.6">
       <c r="B46" s="12"/>
@@ -1931,10 +1950,7 @@
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
       <c r="F51" s="13"/>
-      <c r="G51" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="G51" s="13"/>
       <c r="H51" s="12"/>
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
@@ -2006,15 +2022,7 @@
       <c r="J57" s="12"/>
     </row>
     <row r="58" spans="2:10" ht="15.6">
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
-      <c r="D58" s="12"/>
-      <c r="E58" s="12"/>
-      <c r="F58" s="13"/>
       <c r="G58" s="13"/>
-      <c r="H58" s="12"/>
-      <c r="I58" s="12"/>
-      <c r="J58" s="12"/>
     </row>
     <row r="59" spans="2:10" ht="15.6">
       <c r="G59" s="13"/>
@@ -2045,9 +2053,6 @@
     </row>
     <row r="68" spans="7:7" ht="15.6">
       <c r="G68" s="13"/>
-    </row>
-    <row r="69" spans="7:7" ht="15.6">
-      <c r="G69" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2063,13 +2068,14 @@
     <hyperlink ref="J18" r:id="rId7" xr:uid="{C146487F-8A55-47D0-81A5-1E4ACBF756C1}"/>
     <hyperlink ref="J20" r:id="rId8" xr:uid="{74A76CE5-1740-4604-B4E9-33F5492BEEE7}"/>
     <hyperlink ref="J29" r:id="rId9" xr:uid="{B64613A2-D928-794D-9322-5F41A3F75BA9}"/>
-    <hyperlink ref="J42" r:id="rId10" xr:uid="{89C89E43-E61E-4599-8565-501AE9746EE6}"/>
+    <hyperlink ref="J41" r:id="rId10" xr:uid="{89C89E43-E61E-4599-8565-501AE9746EE6}"/>
     <hyperlink ref="J25" r:id="rId11" xr:uid="{B438B4D8-661B-4982-8181-2CE3940B146D}"/>
     <hyperlink ref="J28" r:id="rId12" xr:uid="{145D90CA-E61E-4FA6-B49C-9DD551BFB85B}"/>
     <hyperlink ref="J27" r:id="rId13" xr:uid="{23C878EF-4344-44FA-B545-AB4F0628BD8E}"/>
-    <hyperlink ref="J45" r:id="rId14" xr:uid="{7597AE0D-2257-4F35-859F-75725C862BA4}"/>
+    <hyperlink ref="J44" r:id="rId14" xr:uid="{7597AE0D-2257-4F35-859F-75725C862BA4}"/>
+    <hyperlink ref="J24" r:id="rId15" xr:uid="{60D605C1-E311-4D18-90BC-17A15D74FD04}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="56" orientation="portrait" r:id="rId15"/>
+  <pageSetup scale="56" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>